<commit_message>
seperated the useful UBPR series and bank in stress-test spreadsheet
</commit_message>
<xml_diff>
--- a/Banks_Participating_in_Stress_Test_by_Year.xlsx
+++ b/Banks_Participating_in_Stress_Test_by_Year.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/59b6ccd87630485b/Duke/Spring_2025/CS590/project/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/59b6ccd87630485b/Duke/Spring_2025/CS590/Dodd-frank-rollback-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:9_{991D5F15-0B4D-457A-B6D2-6FAE1D807CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E4CF89C-A23B-4E68-96FF-112E76B8129F}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="380" windowWidth="20550" windowHeight="12770" xr2:uid="{826C277F-4807-428E-A892-BB0EF606528B}"/>
+    <workbookView xWindow="5" yWindow="5" windowWidth="19190" windowHeight="10790" xr2:uid="{826C277F-4807-428E-A892-BB0EF606528B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -1316,7 +1316,7 @@
   <dimension ref="A1:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
cleaned up stress-test banks list
</commit_message>
<xml_diff>
--- a/Banks_Participating_in_Stress_Test_by_Year.xlsx
+++ b/Banks_Participating_in_Stress_Test_by_Year.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/59b6ccd87630485b/Duke/Spring_2025/CS590/Dodd-frank-rollback-analysis/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="43" documentId="13_ncr:9_{991D5F15-0B4D-457A-B6D2-6FAE1D807CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0E4CF89C-A23B-4E68-96FF-112E76B8129F}"/>
+  <xr:revisionPtr revIDLastSave="91" documentId="13_ncr:9_{991D5F15-0B4D-457A-B6D2-6FAE1D807CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1E55A333-569E-4AC0-9CA1-C5BEE024F5F9}"/>
   <bookViews>
-    <workbookView xWindow="5" yWindow="5" windowWidth="19190" windowHeight="10790" xr2:uid="{826C277F-4807-428E-A892-BB0EF606528B}"/>
+    <workbookView xWindow="-20588" yWindow="-98" windowWidth="20686" windowHeight="15556" xr2:uid="{826C277F-4807-428E-A892-BB0EF606528B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
-    <sheet name="Banks_Participating_in_Stress_T" sheetId="1" r:id="rId2"/>
+    <sheet name="Banks_Participating_in_Stress_T" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -34,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>Banks That Remained in Stress Tests Post the 2018 Roll Back</t>
   </si>
@@ -48,12 +47,6 @@
     <t>Bank of America Corporation</t>
   </si>
   <si>
-    <t>Barclays US LLC</t>
-  </si>
-  <si>
-    <t>BARCLAYS BANK DELAWARE</t>
-  </si>
-  <si>
     <t>Capital One Financial Corporation</t>
   </si>
   <si>
@@ -66,18 +59,6 @@
     <t>CITIBANK, N.A.</t>
   </si>
   <si>
-    <t>Credit Suisse Holdings (USA), Inc.</t>
-  </si>
-  <si>
-    <t>gone</t>
-  </si>
-  <si>
-    <t>DB USA Corporation</t>
-  </si>
-  <si>
-    <t>???</t>
-  </si>
-  <si>
     <t>HSBC North America Holdings Inc.</t>
   </si>
   <si>
@@ -90,21 +71,12 @@
     <t>JPMORGAN CHASE BANK, NATIONAL ASSOCIATION</t>
   </si>
   <si>
-    <t>Morgan Stanley</t>
-  </si>
-  <si>
-    <t>MORGAN STANLEY BANK, N.A., MORGAN STANLEY PRIVATE BANK, NATIONAL ASSOCIATION</t>
-  </si>
-  <si>
     <t>Northern Trust Corporation</t>
   </si>
   <si>
     <t>NORTHERN TRUST COMPANY, THE</t>
   </si>
   <si>
-    <t>State Street Corporation</t>
-  </si>
-  <si>
     <t>TD Group US Holdings LLC</t>
   </si>
   <si>
@@ -135,12 +107,6 @@
     <t>U.S. BANK NATIONAL ASSOCIATION</t>
   </si>
   <si>
-    <t>UBS Americas Holding LLC</t>
-  </si>
-  <si>
-    <t>UBS BANK USA</t>
-  </si>
-  <si>
     <t>Wells Fargo &amp; Company</t>
   </si>
   <si>
@@ -162,27 +128,12 @@
     <t>AMERICAN EXPRESS NATIONAL BANK</t>
   </si>
   <si>
-    <t>BB&amp;T Corporation</t>
-  </si>
-  <si>
-    <t>merged with SunTrust</t>
-  </si>
-  <si>
-    <t>BBVA Compass Bancshares, Inc.</t>
-  </si>
-  <si>
     <t>BMO Financial Corp.</t>
   </si>
   <si>
     <t>BMO BANK NATIONAL ASSOCIATION</t>
   </si>
   <si>
-    <t>BNP Paribas USA, Inc.</t>
-  </si>
-  <si>
-    <t>Citizens Financial Group, Inc.</t>
-  </si>
-  <si>
     <t>Discover Financial Services</t>
   </si>
   <si>
@@ -213,226 +164,23 @@
     <t>MANUFACTURERS AND TRADERS TRUST COMPANY</t>
   </si>
   <si>
-    <t>MUFG Americas Holdings Corporation</t>
-  </si>
-  <si>
-    <t>RBC USA Holdco Corporation</t>
-  </si>
-  <si>
-    <t>RBC BANK (GEORGIA), NATIONAL ASSOCIATION</t>
-  </si>
-  <si>
-    <t>couldn't find the bank that’s holding all the assets</t>
-  </si>
-  <si>
     <t>Regions Financial Corporation</t>
   </si>
   <si>
     <t>REGIONS BANK</t>
   </si>
   <si>
-    <t>Santander Holdings USA, Inc.</t>
-  </si>
-  <si>
-    <t>SANTANDER BANK, NATIONAL ASSOCIATION</t>
-  </si>
-  <si>
-    <t>SunTrust Banks, Inc.</t>
-  </si>
-  <si>
-    <t>merged with BB&amp;T</t>
-  </si>
-  <si>
-    <t>Analysis Theme</t>
-  </si>
-  <si>
-    <t>UBPR Series Code</t>
-  </si>
-  <si>
-    <t>Series Definition / Explanation</t>
-  </si>
-  <si>
-    <t>Liquidity &amp; Investment Portfolio (Page 10A)</t>
-  </si>
-  <si>
-    <t>Liquidity Measures</t>
-  </si>
-  <si>
-    <t>UBPRE589</t>
-  </si>
-  <si>
-    <t>Short Term Investments as % of Total Assets – measures liquid assets (cash equivalents, short-term securities) relative to total assets​</t>
-  </si>
-  <si>
-    <t>Liquidity &amp; Funding (Page 10)</t>
-  </si>
-  <si>
-    <t>UBPRE595</t>
-  </si>
-  <si>
-    <t>Brokered Deposits to Total Deposits – fraction of total deposits obtained through brokers, indicating reliance on wholesale funding​</t>
-  </si>
-  <si>
-    <t>UBPRK447</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Net Non-Core Funding Dependence – non-core liabilities </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>minus</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> short-term investments divided by long-term assets (higher values signal greater reliance on less-stable funding)​</t>
-    </r>
-  </si>
-  <si>
-    <t>UBPRE591</t>
-  </si>
-  <si>
-    <t>Core Deposits as % of Total Assets – share of stable core deposits (demand, savings, insured time deposits) in the bank’s asset funding mix​</t>
-  </si>
-  <si>
-    <t>Summary Ratios (Page 1)</t>
-  </si>
-  <si>
-    <t>Profitability &amp; Earnings Stability</t>
-  </si>
-  <si>
-    <t>UBPRE013</t>
-  </si>
-  <si>
-    <t>Return on Average Assets (ROA) – net income after taxes as a percent of average total assets (overall bank profitability)​</t>
-  </si>
-  <si>
-    <t>Capital Analysis (Page 11)</t>
-  </si>
-  <si>
-    <t>UBPRE630</t>
-  </si>
-  <si>
-    <t>Return on Equity (ROE) – net income as a percent of average total bank equity capital (shareholder return on equity)​</t>
-  </si>
-  <si>
-    <t>UBPRE018</t>
-  </si>
-  <si>
-    <t>Net Interest Margin (NIM) – net interest income (tax-equivalent) as a percent of average earning assets (reflects core spread-based earnings)​</t>
-  </si>
-  <si>
-    <t>UBPRE004</t>
-  </si>
-  <si>
-    <t>Noninterest Income / Average Assets – fee-based and other non-interest income as a percent of average assets (indicates revenue diversification)​</t>
-  </si>
-  <si>
-    <t>Stress Testing Performance</t>
-  </si>
-  <si>
-    <t>UBPR7204</t>
-  </si>
-  <si>
-    <t>Tier 1 Leverage Capital Ratio – Tier 1 capital (core capital) as a percent of average tangible assets (a basic capital buffer measure)​</t>
-  </si>
-  <si>
-    <t>UBPR7206</t>
-  </si>
-  <si>
-    <t>Tier 1 Risk-Based Capital Ratio – Tier 1 capital as a percent of risk-weighted assets (core capital adequacy under risk-based standards)​</t>
-  </si>
-  <si>
-    <t>UBPR7205</t>
-  </si>
-  <si>
-    <t>Total Risk-Based Capital Ratio – total regulatory capital (Tier 1 + Tier 2) as a percent of risk-weighted assets (overall capital cushion above minimum requirements)​</t>
-  </si>
-  <si>
-    <t>Loan Mix (Page 7A)</t>
-  </si>
-  <si>
-    <t>Consumer &amp; Small Business Lending</t>
-  </si>
-  <si>
-    <t>UBPRE415</t>
-  </si>
-  <si>
-    <t>1–4 Family Residential Loans (% Gross Loans) – portion of the loan portfolio invested in residential mortgage loans (home lending)​</t>
-  </si>
-  <si>
-    <t>UBPRE424</t>
-  </si>
-  <si>
-    <t>Loans to Individuals (% Gross Loans) – share of total loans made to consumers for household, family, and personal needs (includes credit card, auto, etc.)​</t>
-  </si>
-  <si>
-    <t>UBPRE423</t>
-  </si>
-  <si>
-    <t>Commercial &amp; Industrial Loans (% Gross Loans) – percentage of the loan book devoted to C&amp;I loans (business lending, a proxy for small business credit in many banks)​</t>
-  </si>
-  <si>
-    <t>Noninterest Income &amp; Expense (Page 3)</t>
-  </si>
-  <si>
-    <t>Compliance Costs &amp; Operational Changes</t>
-  </si>
-  <si>
-    <t>UBPRE005</t>
-  </si>
-  <si>
-    <t>Non-Interest Expense / Average Assets – total overhead operating expense as a percent of average assets (captures overall operating costs, including compliance-related expenses)​</t>
-  </si>
-  <si>
-    <t>UBPRE088</t>
-  </si>
-  <si>
-    <t>Efficiency Ratio – total overhead expense expressed as a percentage of net interest income (TE) plus noninterest income (gauges cost efficiency and burden of compliance/operations)​</t>
-  </si>
-  <si>
-    <t>Capital Analysis-a (Page 11)</t>
-  </si>
-  <si>
-    <t>FFIEC CDR UBPR Ratios Concept Not In Presentation 2002</t>
-  </si>
-  <si>
-    <t>FFIEC CDR UBPR Ratios Concept Not In Presentation 2003</t>
-  </si>
-  <si>
-    <t>FFIEC CDR UBPR Ratios Concept Not In Presentation 2004</t>
-  </si>
-  <si>
-    <t>combined</t>
-  </si>
-  <si>
     <t>BANK OF AMERICA, NATIONAL ASSOCIATION</t>
   </si>
   <si>
-    <t>UBPR User Guide File</t>
-  </si>
-  <si>
-    <t>Data File</t>
+    <t>Note:  all the below banks are removed from stress test in 2018, but once again subjected to DFAST 2020 and onwards</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -568,15 +316,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
-      <sz val="11"/>
+      <b/>
+      <sz val="16"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -923,16 +665,18 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="42">
@@ -990,10 +734,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1312,676 +1052,274 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4CD8550D-585E-4AE4-9E1C-7A6C968618A4}">
-  <dimension ref="A1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA653223-556B-4AF6-9C8F-DBC537FCF225}">
+  <dimension ref="A1:C25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.1796875" customWidth="1"/>
-    <col min="3" max="3" width="11.36328125" customWidth="1"/>
-    <col min="4" max="4" width="62.6328125" customWidth="1"/>
-    <col min="5" max="5" width="48.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="74.7265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="50.54296875" customWidth="1"/>
+    <col min="3" max="3" width="10.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="21" x14ac:dyDescent="0.5">
       <c r="A1" s="1" t="s">
-        <v>121</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A3" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="E3" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>98</v>
-      </c>
-      <c r="E4" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>94</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="E5" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="43.5" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A8" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A13" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="87" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A15" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="58" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="58" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>84</v>
-      </c>
-      <c r="C17" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>93</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D17">
-    <sortCondition ref="A2:A17"/>
-  </sortState>
-  <phoneticPr fontId="19" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA653223-556B-4AF6-9C8F-DBC537FCF225}">
-  <dimension ref="A1:D39"/>
-  <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="24.54296875" customWidth="1"/>
-    <col min="2" max="2" width="38" customWidth="1"/>
-    <col min="3" max="3" width="29.54296875" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>120</v>
+      <c r="B2" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="C2">
         <v>480228</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="3" t="s">
         <v>5</v>
       </c>
       <c r="C3">
-        <v>2980209</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+        <v>112837</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C4">
-        <v>112837</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+        <v>476810</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>8</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C5">
-        <v>476810</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+        <v>413208</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>10</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C6">
+        <v>852218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>12</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C7">
+        <v>210434</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C8">
-        <v>413208</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+        <v>2121196</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>16</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B9" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C9">
-        <v>852218</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+        <v>541101</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C10">
-        <v>1456501</v>
-      </c>
-      <c r="D10">
-        <v>2489805</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+        <v>2182786</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>20</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
       <c r="C11">
-        <v>210434</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+        <v>817824</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>22</v>
       </c>
-      <c r="B12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12">
+        <v>504713</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>23</v>
-      </c>
-      <c r="B13" t="s">
         <v>24</v>
       </c>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
       <c r="C13">
-        <v>2121196</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>25</v>
-      </c>
-      <c r="B14" t="s">
+        <v>451965</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B14" s="3"/>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16" spans="1:3" ht="30.5" x14ac:dyDescent="0.5">
+      <c r="A16" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C14">
-        <v>541101</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" t="s">
+      <c r="B16" s="5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C15">
-        <v>2182786</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" t="s">
+      <c r="C17" s="2">
+        <v>3284070</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B18" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C16">
-        <v>817824</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A17" t="s">
+      <c r="C18" s="2">
+        <v>1394676</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B19" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C17">
-        <v>504713</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A18" t="s">
+      <c r="C19" s="2">
+        <v>75633</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B20" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="C18">
-        <v>3212149</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A19" t="s">
+      <c r="C20" s="2">
+        <v>30810</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B21" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="C19">
-        <v>451965</v>
+      <c r="C21" s="2">
+        <v>723112</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" t="s">
+      <c r="A22" s="2" t="s">
         <v>37</v>
       </c>
+      <c r="B22" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="C22" s="2">
+        <v>12311</v>
+      </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A23" t="s">
-        <v>38</v>
-      </c>
-      <c r="B23" t="s">
+      <c r="A23" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C23">
-        <v>3284070</v>
+      <c r="B23" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="2">
+        <v>280110</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A24" t="s">
-        <v>40</v>
-      </c>
-      <c r="B24" t="s">
+      <c r="A24" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C24">
-        <v>1394676</v>
+      <c r="B24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C24" s="2">
+        <v>501105</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" t="s">
-        <v>42</v>
-      </c>
-      <c r="B25" t="s">
+      <c r="A25" s="2" t="s">
         <v>43</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A26" t="s">
+      <c r="B25" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="B26" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A27" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" t="s">
-        <v>46</v>
-      </c>
-      <c r="C27">
-        <v>75633</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A28" t="s">
-        <v>47</v>
-      </c>
-      <c r="B28" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A30" t="s">
-        <v>49</v>
-      </c>
-      <c r="B30" t="s">
-        <v>50</v>
-      </c>
-      <c r="C30">
-        <v>30810</v>
-      </c>
-    </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A31" t="s">
-        <v>51</v>
-      </c>
-      <c r="B31" t="s">
-        <v>52</v>
-      </c>
-      <c r="C31">
-        <v>723112</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A32" t="s">
-        <v>53</v>
-      </c>
-      <c r="B32" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32">
-        <v>12311</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A33" t="s">
-        <v>55</v>
-      </c>
-      <c r="B33" t="s">
-        <v>56</v>
-      </c>
-      <c r="C33">
-        <v>280110</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A34" t="s">
-        <v>57</v>
-      </c>
-      <c r="B34" t="s">
-        <v>58</v>
-      </c>
-      <c r="C34">
-        <v>501105</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A35" t="s">
-        <v>59</v>
-      </c>
-      <c r="B35" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A36" t="s">
-        <v>60</v>
-      </c>
-      <c r="B36" t="s">
-        <v>61</v>
-      </c>
-      <c r="C36">
-        <v>3783948</v>
-      </c>
-      <c r="D36" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A37" t="s">
-        <v>63</v>
-      </c>
-      <c r="B37" t="s">
-        <v>64</v>
-      </c>
-      <c r="C37">
+      <c r="C25" s="2">
         <v>233031</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A38" t="s">
-        <v>65</v>
-      </c>
-      <c r="B38" t="s">
-        <v>66</v>
-      </c>
-      <c r="C38">
-        <v>722777</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A39" t="s">
-        <v>67</v>
-      </c>
-      <c r="B39" t="s">
-        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>